<commit_message>
updated slideshow, guest list
</commit_message>
<xml_diff>
--- a/sql/Wedding Guest List_v2_161007.xlsx
+++ b/sql/Wedding Guest List_v2_161007.xlsx
@@ -2449,12 +2449,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +2496,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>146</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>256</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>257</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>229</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>181</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>190</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>157</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>158</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>168</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>154</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>156</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>206</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>207</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>469</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>470</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>354</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>254</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>251</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>471</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>216</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>204</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>246</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>614</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>223</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>224</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>197</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>242</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>149</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>205</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>203</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>163</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>179</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>152</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>153</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>194</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>230</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>185</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>167</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>175</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>407</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>198</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>221</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>171</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>186</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>187</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>159</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>160</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>161</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>251</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>171</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>251</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>182</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>169</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>193</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>248</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>119</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>120</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>150</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>151</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>145</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>178</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>251</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>196</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>192</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>191</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>167</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>220</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>165</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>240</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>151</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>178</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>189</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>202</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>255</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>213</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>214</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>491</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>218</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>219</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>167</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>247</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>167</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>250</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>178</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>184</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>150</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>192</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>160</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>167</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>163</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>487</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>127</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>154</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>222</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>215</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>212</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>251</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>210</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>243</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>177</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>146</v>
       </c>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>677</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>146</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>163</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>211</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>228</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>176</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>2</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>23</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>169</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>170</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>176</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>159</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>2</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>208</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>209</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>195</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>181</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>174</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>179</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>159</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>183</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>149</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>148</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>167</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>188</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>185</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>252</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>237</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>157</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>225</v>
       </c>
@@ -5692,11 +5692,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H155">
-    <filterColumn colId="7">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
     <sortState ref="A6:H151">
       <sortCondition ref="D1:D155"/>
     </sortState>
@@ -5712,7 +5707,7 @@
   <dimension ref="A1:J152"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>

</xml_diff>